<commit_message>
add clean target to Makefile
</commit_message>
<xml_diff>
--- a/example.xlsx
+++ b/example.xlsx
@@ -210,11 +210,11 @@
   </sheetPr>
   <dimension ref="A1:I4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I5" activeCellId="0" sqref="I5"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="220" zoomScaleNormal="220" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I4" activeCellId="0" sqref="I4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="7.26"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="10.6"/>

</xml_diff>